<commit_message>
cambio en la base de datos, se agregaron campos en todos los contratos
</commit_message>
<xml_diff>
--- a/consulta/co/contrato_de_obra.xlsx
+++ b/consulta/co/contrato_de_obra.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18915" windowHeight="8505"/>
+    <workbookView xWindow="-15" yWindow="105" windowWidth="19590" windowHeight="4245"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,20 +31,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="General_)"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,18 +41,30 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -78,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -86,56 +85,47 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="12">
-    <cellStyle name="=C:\WINNT\SYSTEM32\COMMAND.COM" xfId="1"/>
-    <cellStyle name="=C:\WINNT\SYSTEM32\COMMAND.COM 2" xfId="2"/>
-    <cellStyle name="=C:\WINNT\SYSTEM32\COMMAND.COM 2 2" xfId="3"/>
-    <cellStyle name="Millares 2" xfId="4"/>
-    <cellStyle name="Moneda 2" xfId="5"/>
-    <cellStyle name="Moneda 2 2 3" xfId="6"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="7"/>
-    <cellStyle name="Normal 2 2" xfId="8"/>
-    <cellStyle name="Normal 3" xfId="9"/>
-    <cellStyle name="Normal 4" xfId="10"/>
-    <cellStyle name="Porcentual 2" xfId="11"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -149,42 +139,31 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>142876</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>752476</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>380999</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="2264611" cy="1152525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3952876" y="114300"/>
-          <a:ext cx="2133600" cy="1085849"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2264611" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -192,7 +171,40 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2264611" cy="1152525"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8124825" y="28575"/>
+          <a:ext cx="2264611" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -483,49 +495,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H6"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:44" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:44" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
     </row>
-    <row r="3" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:44" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+    <row r="5" spans="1:44" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>